<commit_message>
Added Updated Object Repository
Added Updated Object Repository
</commit_message>
<xml_diff>
--- a/SampleScript/TestOR/DemoOR.xlsx
+++ b/SampleScript/TestOR/DemoOR.xlsx
@@ -2,19 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="hidden" xWindow="-105" yWindow="2145" windowWidth="28830" windowHeight="4545"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$12</definedName>
-  </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
@@ -36,91 +33,91 @@
     <t>ObjectPath</t>
   </si>
   <si>
+    <t>TxtSearch</t>
+  </si>
+  <si>
+    <t>Textbox</t>
+  </si>
+  <si>
+    <t>id=lst-ib</t>
+  </si>
+  <si>
+    <t>BtnSearch</t>
+  </si>
+  <si>
     <t>Button</t>
   </si>
   <si>
-    <t>Textbox</t>
+    <t>xpath=//*[@id="sblsbb"]/button/span</t>
+  </si>
+  <si>
+    <t>linkO2t</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>xpath=//*[@id="rso"]/div[1]/div/div/h3/a</t>
+  </si>
+  <si>
+    <t>linkComments</t>
+  </si>
+  <si>
+    <t>xpath=/html/body/div[1]/div[1]/div/div/a[6]</t>
+  </si>
+  <si>
+    <t>TxtName</t>
   </si>
   <si>
     <t>textbox</t>
   </si>
   <si>
+    <t>name=cname</t>
+  </si>
+  <si>
     <t>TxtEmail</t>
   </si>
   <si>
-    <t>TxtName</t>
+    <t>name=cemailID</t>
+  </si>
+  <si>
+    <t>TxtCompany</t>
+  </si>
+  <si>
+    <t>name=corganization</t>
   </si>
   <si>
     <t>ListSource</t>
   </si>
   <si>
-    <t>name=cname</t>
-  </si>
-  <si>
-    <t>name=cemailID</t>
-  </si>
-  <si>
-    <t>name=corganization</t>
+    <t>combobox</t>
   </si>
   <si>
     <t>id=select</t>
   </si>
   <si>
+    <t>Listitem</t>
+  </si>
+  <si>
+    <t>xpath=//*[@id="select"]/option[7]</t>
+  </si>
+  <si>
+    <t>TxtComments</t>
+  </si>
+  <si>
+    <t>Textarea</t>
+  </si>
+  <si>
     <t>id=comments</t>
   </si>
   <si>
-    <t>TxtCompany</t>
-  </si>
-  <si>
-    <t>TxtComments</t>
-  </si>
-  <si>
-    <t>Textarea</t>
-  </si>
-  <si>
-    <t>id=lst-ib</t>
-  </si>
-  <si>
-    <t>TxtSearch</t>
-  </si>
-  <si>
-    <t>xpath=//*[@id="sblsbb"]/button/span</t>
-  </si>
-  <si>
-    <t>BtnSearch</t>
-  </si>
-  <si>
-    <t>xpath=//*[@id="rso"]/div[1]/div/div/h3/a</t>
-  </si>
-  <si>
-    <t>linkO2t</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>xpath=/html/body/div[1]/div[1]/div/div/a[6]</t>
-  </si>
-  <si>
-    <t>linkComments</t>
-  </si>
-  <si>
-    <t>xpath=//*[@id="select"]/option[7]</t>
-  </si>
-  <si>
-    <t>Listitem</t>
-  </si>
-  <si>
-    <t>combobox</t>
+    <t>submitForm</t>
+  </si>
+  <si>
+    <t>button</t>
   </si>
   <si>
     <t>xpath=//*[@id="contribute"]/img</t>
-  </si>
-  <si>
-    <t>button</t>
-  </si>
-  <si>
-    <t>submitForm</t>
   </si>
   <si>
     <t>xpath=//*[@id="comments"]</t>
@@ -130,23 +127,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="128"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,12 +146,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -191,35 +175,30 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -517,20 +496,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,215 +527,212 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="2" customFormat="1">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="3">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="2" customFormat="1">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="s">
+    </row>
+    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="B12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="2" customFormat="1">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="2" customFormat="1">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="2" customFormat="1">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="2" customFormat="1">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="2" customFormat="1">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="6">
-        <v>1</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E12"/>
-  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -765,9 +742,8 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -778,9 +754,8 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>